<commit_message>
Update PS table for rate studies 2018_v2_1_0
</commit_message>
<xml_diff>
--- a/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-DedicatedRateStudy.xlsx
+++ b/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-DedicatedRateStudy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709743F5-1DF5-E24E-BCD6-EB929B2055D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36A85C6-F3F1-354D-8495-65580BE656B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28620" windowHeight="16600" xr2:uid="{D43503D0-D942-054C-A252-8EF60B2ECDE6}"/>
+    <workbookView xWindow="-40" yWindow="-20380" windowWidth="30580" windowHeight="17280" xr2:uid="{D43503D0-D942-054C-A252-8EF60B2ECDE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1079,7 +1079,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1091,6 +1091,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1143,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1152,6 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46014C27-F11A-2A41-BE5F-BBB4784EB01D}">
   <dimension ref="A1:O344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="H348" sqref="H348"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1496,7 @@
       <c r="C1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="3">
         <v>1.9999999999999999E+34</v>
       </c>
       <c r="E1" s="3">
@@ -2431,11 +2439,11 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -2452,8 +2460,8 @@
       <c r="K21" s="1">
         <v>1</v>
       </c>
-      <c r="L21" s="4">
-        <v>0</v>
+      <c r="L21" s="1">
+        <v>1</v>
       </c>
       <c r="M21" s="4">
         <v>0</v>
@@ -3888,8 +3896,8 @@
       <c r="D52" s="1">
         <v>2</v>
       </c>
-      <c r="E52" s="1">
-        <v>2</v>
+      <c r="E52" s="8">
+        <v>50</v>
       </c>
       <c r="F52" s="1">
         <v>2</v>
@@ -3912,14 +3920,14 @@
       <c r="L52" s="1">
         <v>2</v>
       </c>
-      <c r="M52" s="1">
-        <v>2</v>
-      </c>
-      <c r="N52" s="1">
-        <v>2</v>
-      </c>
-      <c r="O52" s="1">
-        <v>2</v>
+      <c r="M52" s="8">
+        <v>50</v>
+      </c>
+      <c r="N52" s="8">
+        <v>50</v>
+      </c>
+      <c r="O52" s="8">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -7416,8 +7424,8 @@
       <c r="E127" s="1">
         <v>1</v>
       </c>
-      <c r="F127" s="4">
-        <v>0</v>
+      <c r="F127" s="1">
+        <v>1</v>
       </c>
       <c r="G127" s="4">
         <v>0</v>
@@ -7434,8 +7442,8 @@
       <c r="K127" s="1">
         <v>1</v>
       </c>
-      <c r="L127" s="4">
-        <v>0</v>
+      <c r="L127" s="1">
+        <v>1</v>
       </c>
       <c r="M127" s="4">
         <v>0</v>
@@ -7466,8 +7474,8 @@
       <c r="F128" s="1">
         <v>1</v>
       </c>
-      <c r="G128" s="4">
-        <v>0</v>
+      <c r="G128" s="1">
+        <v>1</v>
       </c>
       <c r="H128" s="1">
         <v>1</v>
@@ -7484,8 +7492,8 @@
       <c r="L128" s="1">
         <v>1</v>
       </c>
-      <c r="M128" s="4">
-        <v>0</v>
+      <c r="M128" s="1">
+        <v>1</v>
       </c>
       <c r="N128" s="1">
         <v>1</v>
@@ -7787,39 +7795,39 @@
         <v>0</v>
       </c>
       <c r="D135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" s="1">
-        <v>0</v>
-      </c>
-      <c r="G135" s="1">
-        <v>0</v>
-      </c>
-      <c r="H135" s="1">
-        <v>0</v>
-      </c>
-      <c r="I135" s="1">
+        <v>1</v>
+      </c>
+      <c r="G135" s="4">
+        <v>0</v>
+      </c>
+      <c r="H135" s="4">
+        <v>0</v>
+      </c>
+      <c r="I135" s="4">
         <v>0</v>
       </c>
       <c r="J135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L135" s="1">
-        <v>0</v>
-      </c>
-      <c r="M135" s="1">
-        <v>0</v>
-      </c>
-      <c r="N135" s="1">
-        <v>0</v>
-      </c>
-      <c r="O135" s="1">
+        <v>1</v>
+      </c>
+      <c r="M135" s="4">
+        <v>0</v>
+      </c>
+      <c r="N135" s="4">
+        <v>0</v>
+      </c>
+      <c r="O135" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7886,8 +7894,8 @@
       <c r="E137" s="1">
         <v>1</v>
       </c>
-      <c r="F137" s="4">
-        <v>0</v>
+      <c r="F137" s="1">
+        <v>1</v>
       </c>
       <c r="G137" s="4">
         <v>0</v>
@@ -7904,8 +7912,8 @@
       <c r="K137" s="1">
         <v>1</v>
       </c>
-      <c r="L137" s="4">
-        <v>0</v>
+      <c r="L137" s="1">
+        <v>1</v>
       </c>
       <c r="M137" s="4">
         <v>0</v>
@@ -7933,8 +7941,8 @@
       <c r="E138" s="1">
         <v>1</v>
       </c>
-      <c r="F138" s="4">
-        <v>0</v>
+      <c r="F138" s="1">
+        <v>1</v>
       </c>
       <c r="G138" s="4">
         <v>0</v>
@@ -7951,8 +7959,8 @@
       <c r="K138" s="1">
         <v>1</v>
       </c>
-      <c r="L138" s="4">
-        <v>0</v>
+      <c r="L138" s="1">
+        <v>1</v>
       </c>
       <c r="M138" s="4">
         <v>0</v>
@@ -8403,8 +8411,8 @@
       <c r="E148" s="1">
         <v>1</v>
       </c>
-      <c r="F148" s="4">
-        <v>0</v>
+      <c r="F148" s="1">
+        <v>1</v>
       </c>
       <c r="G148" s="4">
         <v>0</v>
@@ -8421,8 +8429,8 @@
       <c r="K148" s="1">
         <v>1</v>
       </c>
-      <c r="L148" s="4">
-        <v>0</v>
+      <c r="L148" s="1">
+        <v>1</v>
       </c>
       <c r="M148" s="4">
         <v>0</v>
@@ -8450,8 +8458,8 @@
       <c r="E149" s="1">
         <v>1</v>
       </c>
-      <c r="F149" s="4">
-        <v>0</v>
+      <c r="F149" s="1">
+        <v>1</v>
       </c>
       <c r="G149" s="4">
         <v>0</v>
@@ -8468,8 +8476,8 @@
       <c r="K149" s="1">
         <v>1</v>
       </c>
-      <c r="L149" s="4">
-        <v>0</v>
+      <c r="L149" s="1">
+        <v>1</v>
       </c>
       <c r="M149" s="4">
         <v>0</v>
@@ -8497,8 +8505,8 @@
       <c r="E150" s="1">
         <v>1</v>
       </c>
-      <c r="F150" s="4">
-        <v>0</v>
+      <c r="F150" s="1">
+        <v>1</v>
       </c>
       <c r="G150" s="4">
         <v>0</v>
@@ -8515,8 +8523,8 @@
       <c r="K150" s="1">
         <v>1</v>
       </c>
-      <c r="L150" s="4">
-        <v>0</v>
+      <c r="L150" s="1">
+        <v>1</v>
       </c>
       <c r="M150" s="4">
         <v>0</v>
@@ -8547,8 +8555,8 @@
       <c r="F151" s="1">
         <v>1</v>
       </c>
-      <c r="G151" s="4">
-        <v>0</v>
+      <c r="G151" s="1">
+        <v>1</v>
       </c>
       <c r="H151" s="1">
         <v>1</v>
@@ -8565,8 +8573,8 @@
       <c r="L151" s="1">
         <v>1</v>
       </c>
-      <c r="M151" s="4">
-        <v>0</v>
+      <c r="M151" s="1">
+        <v>1</v>
       </c>
       <c r="N151" s="1">
         <v>1</v>
@@ -8594,8 +8602,8 @@
       <c r="F152" s="1">
         <v>1</v>
       </c>
-      <c r="G152" s="4">
-        <v>0</v>
+      <c r="G152" s="1">
+        <v>1</v>
       </c>
       <c r="H152" s="1">
         <v>1</v>
@@ -8612,8 +8620,8 @@
       <c r="L152" s="1">
         <v>1</v>
       </c>
-      <c r="M152" s="4">
-        <v>0</v>
+      <c r="M152" s="1">
+        <v>1</v>
       </c>
       <c r="N152" s="1">
         <v>1</v>
@@ -9766,8 +9774,8 @@
       <c r="E177" s="1">
         <v>1</v>
       </c>
-      <c r="F177" s="4">
-        <v>0</v>
+      <c r="F177" s="1">
+        <v>1</v>
       </c>
       <c r="G177" s="4">
         <v>0</v>
@@ -9784,8 +9792,8 @@
       <c r="K177" s="1">
         <v>1</v>
       </c>
-      <c r="L177" s="4">
-        <v>0</v>
+      <c r="L177" s="1">
+        <v>1</v>
       </c>
       <c r="M177" s="4">
         <v>0</v>
@@ -9907,8 +9915,8 @@
       <c r="E180" s="1">
         <v>1</v>
       </c>
-      <c r="F180" s="4">
-        <v>0</v>
+      <c r="F180" s="1">
+        <v>1</v>
       </c>
       <c r="G180" s="4">
         <v>0</v>
@@ -9925,8 +9933,8 @@
       <c r="K180" s="1">
         <v>1</v>
       </c>
-      <c r="L180" s="4">
-        <v>0</v>
+      <c r="L180" s="1">
+        <v>1</v>
       </c>
       <c r="M180" s="4">
         <v>0</v>
@@ -9957,8 +9965,8 @@
       <c r="F181" s="1">
         <v>1</v>
       </c>
-      <c r="G181" s="4">
-        <v>0</v>
+      <c r="G181" s="1">
+        <v>1</v>
       </c>
       <c r="H181" s="4">
         <v>0</v>
@@ -9975,8 +9983,8 @@
       <c r="L181" s="1">
         <v>1</v>
       </c>
-      <c r="M181" s="4">
-        <v>0</v>
+      <c r="M181" s="1">
+        <v>1</v>
       </c>
       <c r="N181" s="4">
         <v>0</v>
@@ -10283,8 +10291,8 @@
       <c r="E188" s="1">
         <v>1</v>
       </c>
-      <c r="F188" s="4">
-        <v>0</v>
+      <c r="F188" s="1">
+        <v>1</v>
       </c>
       <c r="G188" s="4">
         <v>0</v>
@@ -10301,8 +10309,8 @@
       <c r="K188" s="1">
         <v>1</v>
       </c>
-      <c r="L188" s="4">
-        <v>0</v>
+      <c r="L188" s="1">
+        <v>1</v>
       </c>
       <c r="M188" s="4">
         <v>0</v>
@@ -10677,8 +10685,8 @@
       <c r="K196" s="1">
         <v>1</v>
       </c>
-      <c r="L196" s="4">
-        <v>0</v>
+      <c r="L196" s="1">
+        <v>1</v>
       </c>
       <c r="M196" s="4">
         <v>0</v>
@@ -10724,7 +10732,7 @@
       <c r="K197" s="1">
         <v>1</v>
       </c>
-      <c r="L197" s="5">
+      <c r="L197" s="1">
         <v>1</v>
       </c>
       <c r="M197" s="5">
@@ -11852,8 +11860,8 @@
       <c r="K221" s="4">
         <v>0</v>
       </c>
-      <c r="L221" s="4">
-        <v>0</v>
+      <c r="L221" s="1">
+        <v>1</v>
       </c>
       <c r="M221" s="4">
         <v>0</v>
@@ -12228,8 +12236,8 @@
       <c r="K229" s="4">
         <v>0</v>
       </c>
-      <c r="L229" s="4">
-        <v>0</v>
+      <c r="L229" s="1">
+        <v>1</v>
       </c>
       <c r="M229" s="4">
         <v>0</v>
@@ -12886,8 +12894,8 @@
       <c r="K243" s="4">
         <v>0</v>
       </c>
-      <c r="L243" s="4">
-        <v>0</v>
+      <c r="L243" s="1">
+        <v>1</v>
       </c>
       <c r="M243" s="4">
         <v>0</v>
@@ -13168,8 +13176,8 @@
       <c r="K249" s="4">
         <v>0</v>
       </c>
-      <c r="L249" s="4">
-        <v>0</v>
+      <c r="L249" s="1">
+        <v>1</v>
       </c>
       <c r="M249" s="4">
         <v>0</v>
@@ -13450,8 +13458,8 @@
       <c r="K255" s="1">
         <v>1</v>
       </c>
-      <c r="L255" s="1">
-        <v>1</v>
+      <c r="L255" s="4">
+        <v>0</v>
       </c>
       <c r="M255" s="1">
         <v>1</v>
@@ -13497,8 +13505,8 @@
       <c r="K256" s="1">
         <v>1</v>
       </c>
-      <c r="L256" s="1">
-        <v>1</v>
+      <c r="L256" s="4">
+        <v>0</v>
       </c>
       <c r="M256" s="1">
         <v>1</v>
@@ -13826,8 +13834,8 @@
       <c r="K263" s="4">
         <v>0</v>
       </c>
-      <c r="L263" s="4">
-        <v>0</v>
+      <c r="L263" s="1">
+        <v>1</v>
       </c>
       <c r="M263" s="4">
         <v>0</v>
@@ -14108,8 +14116,8 @@
       <c r="K269" s="4">
         <v>0</v>
       </c>
-      <c r="L269" s="4">
-        <v>0</v>
+      <c r="L269" s="1">
+        <v>1</v>
       </c>
       <c r="M269" s="4">
         <v>0</v>
@@ -14531,8 +14539,8 @@
       <c r="K278" s="4">
         <v>0</v>
       </c>
-      <c r="L278" s="4">
-        <v>0</v>
+      <c r="L278" s="1">
+        <v>1</v>
       </c>
       <c r="M278" s="4">
         <v>0</v>
@@ -17648,5 +17656,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>